<commit_message>
Adicionado o contexto de testes com PicoContainer
</commit_message>
<xml_diff>
--- a/src/main/resources/data/testdata.XLSX
+++ b/src/main/resources/data/testdata.XLSX
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\git\treinamento\automacaoweb\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willian.costa\Documents\eclipse-ws\TREINAMENTO\automacaoweb\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5864E06-292F-4D79-A0F3-D3E7F61C2AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C7BD1-7650-4377-96C7-1AEF55846F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1200" windowWidth="10365" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5535" yWindow="1545" windowWidth="10365" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>

</xml_diff>